<commit_message>
Fix the misplacement of imported blank line annotation #98
</commit_message>
<xml_diff>
--- a/src/Magicodes.ExporterAndImporter.Tests/TestFiles/Import/单列导入测试.xlsx
+++ b/src/Magicodes.ExporterAndImporter.Tests/TestFiles/Import/单列导入测试.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Magicodes.ExporterAndImporter\src\Magicodes.ExporterAndImporter.Tests\TestFiles\Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Person\HueiFeng\Magicodes.IE\src\Magicodes.ExporterAndImporter.Tests\TestFiles\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A345EE0-C694-406B-8928-5C9454AC67D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887459B4-ED53-4E9E-BABB-AA51CCEB10E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="3225" windowWidth="15750" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="导入数据" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>姓名</t>
   </si>
@@ -71,13 +71,17 @@
   </si>
   <si>
     <t>祝科昌</t>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -105,6 +109,12 @@
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -153,7 +163,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -163,6 +173,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -480,94 +493,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" s="1">
+        <v>20190901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -580,5 +600,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>